<commit_message>
I have added new class(Sample Test)
</commit_message>
<xml_diff>
--- a/src/main/java/com/facebook/testdata/FacebookCreateAcountData.xlsx
+++ b/src/main/java/com/facebook/testdata/FacebookCreateAcountData.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2115" windowWidth="14970" windowHeight="6855" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11295" windowHeight="5265"/>
   </bookViews>
   <sheets>
-    <sheet name="NewContacts" sheetId="1" r:id="rId1"/>
-    <sheet name="CreateNewContact" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:F16"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Jack</t>
   </si>
@@ -132,9 +130,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -460,196 +457,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>31218</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>23969</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>31218</v>
       </c>
-      <c r="F4" s="3"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="4">
-        <v>31218</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="4">
-        <v>23969</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4">
-        <v>31218</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -661,16 +558,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>